<commit_message>
Added QA2Profile to Virtual Terminal Test Cases.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/VT-ACH-Data.xlsx
+++ b/KatalonData/Bootstrap/VT-ACH-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FFA061-B164-4DF0-854A-48B78341EAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A3F5AC-2E4B-4CD5-B07E-81D79B4218F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="884" xr2:uid="{3836B69F-85F5-4D65-8F1B-FC37FA075D01}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="884" firstSheet="12" activeTab="17" xr2:uid="{3836B69F-85F5-4D65-8F1B-FC37FA075D01}"/>
   </bookViews>
   <sheets>
     <sheet name="VT-ACHPersonal-NoCF-Generic" sheetId="1" r:id="rId1"/>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C179FDD-E618-4742-8F86-80396375312B}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,6 +1301,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1541,6 +1544,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1781,6 +1787,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2021,6 +2030,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2541,6 +2553,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2548,7 +2563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36AC063-7B2D-4A8C-BBEE-74EC43C855B0}">
   <dimension ref="A1:AI5"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1:AI5"/>
     </sheetView>
   </sheetViews>
@@ -3076,6 +3091,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3596,6 +3614,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3836,6 +3857,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3843,7 +3867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EFF342-4D5E-4066-AB33-FA77D4DA0448}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AH21" sqref="AH21"/>
     </sheetView>
   </sheetViews>
@@ -4082,6 +4106,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -4089,8 +4116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819298FE-667E-4491-B43C-4C5F5C5B86A9}">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4322,6 +4349,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -4329,8 +4359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3208BD3-C71F-4161-AC24-4C1B9A477B93}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="N1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4843,6 +4873,9 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -5364,6 +5397,9 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -5604,6 +5640,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -5845,6 +5884,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -5852,7 +5894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8BAD15-65CA-4065-BED2-481F29154B92}">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -6085,6 +6127,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -6605,6 +6650,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -7125,6 +7173,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -7645,5 +7696,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Personal_SearchTransaction_Generic_TC and Test Data.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/VT-ACH-Data.xlsx
+++ b/KatalonData/Bootstrap/VT-ACH-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A3F5AC-2E4B-4CD5-B07E-81D79B4218F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09440230-F0D8-4CA9-A661-3B92E10F5CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="884" firstSheet="12" activeTab="17" xr2:uid="{3836B69F-85F5-4D65-8F1B-FC37FA075D01}"/>
+    <workbookView minimized="1" xWindow="30780" yWindow="1425" windowWidth="24525" windowHeight="14010" tabRatio="884" xr2:uid="{3836B69F-85F5-4D65-8F1B-FC37FA075D01}"/>
   </bookViews>
   <sheets>
     <sheet name="VT-ACHPersonal-NoCF-Generic" sheetId="1" r:id="rId1"/>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C179FDD-E618-4742-8F86-80396375312B}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4116,7 +4116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819298FE-667E-4491-B43C-4C5F5C5B86A9}">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
VT_Payment Test cases added in Production Verification Script
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/VT-ACH-Data.xlsx
+++ b/KatalonData/Bootstrap/VT-ACH-Data.xlsx
@@ -1,40 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09440230-F0D8-4CA9-A661-3B92E10F5CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{09440230-F0D8-4CA9-A661-3B92E10F5CF2}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="30780" yWindow="1425" windowWidth="24525" windowHeight="14010" tabRatio="884" xr2:uid="{3836B69F-85F5-4D65-8F1B-FC37FA075D01}"/>
+    <workbookView minimized="1" tabRatio="884" windowHeight="14010" windowWidth="24525" xWindow="30780" xr2:uid="{3836B69F-85F5-4D65-8F1B-FC37FA075D01}" yWindow="1425"/>
   </bookViews>
   <sheets>
-    <sheet name="VT-ACHPersonal-NoCF-Generic" sheetId="1" r:id="rId1"/>
-    <sheet name="VT-ACHPersonal-SingleCF-Generic" sheetId="3" r:id="rId2"/>
-    <sheet name="VT-ACHPersonal-DualCF-Generic" sheetId="4" r:id="rId3"/>
-    <sheet name="VT-ACHCorp-NoCF-Generic" sheetId="5" r:id="rId4"/>
-    <sheet name="VT-ACHCorp-SingleCF-Generic" sheetId="6" r:id="rId5"/>
-    <sheet name="VT-ACHCorp-DualCF-Generic" sheetId="7" r:id="rId6"/>
-    <sheet name="VT-P-DebitVoid-NoCF-Generic" sheetId="8" r:id="rId7"/>
-    <sheet name="VT-P-DebitVoid-SingleCF-Generic" sheetId="9" r:id="rId8"/>
-    <sheet name="VT-P-DebitVoid-DualCF-Generic" sheetId="10" r:id="rId9"/>
-    <sheet name="VT-C-DebitVoid-NoCF-Generic" sheetId="11" r:id="rId10"/>
-    <sheet name="VT-C-DebitVoid-SingleCF-Generic" sheetId="12" r:id="rId11"/>
-    <sheet name="VT-C-DebitVoid-DualCF-Generic" sheetId="13" r:id="rId12"/>
-    <sheet name="VT-P-DebitCredit-NoCF-Generic" sheetId="14" r:id="rId13"/>
-    <sheet name="VT-P-DebitCredit-SingleCF-Gener" sheetId="15" r:id="rId14"/>
-    <sheet name="VT-P-DebitCredit-DualCF-Generic" sheetId="16" r:id="rId15"/>
-    <sheet name="VT-C-DebitCredit-NoCF-Generic" sheetId="17" r:id="rId16"/>
-    <sheet name="VT-C-DebitCredit-SingleCF-Gener" sheetId="18" r:id="rId17"/>
-    <sheet name="VT-C-DebitCredit-DualCF-Generic" sheetId="19" r:id="rId18"/>
+    <sheet name="VT-ACHPersonal-NoCF-Generic" r:id="rId1" sheetId="1"/>
+    <sheet name="VT-ACHPersonal-SingleCF-Generic" r:id="rId2" sheetId="3"/>
+    <sheet name="VT-ACHPersonal-DualCF-Generic" r:id="rId3" sheetId="4"/>
+    <sheet name="VT-ACHCorp-NoCF-Generic" r:id="rId4" sheetId="5"/>
+    <sheet name="VT-ACHCorp-SingleCF-Generic" r:id="rId5" sheetId="6"/>
+    <sheet name="VT-ACHCorp-DualCF-Generic" r:id="rId6" sheetId="7"/>
+    <sheet name="VT-P-DebitVoid-NoCF-Generic" r:id="rId7" sheetId="8"/>
+    <sheet name="VT-P-DebitVoid-SingleCF-Generic" r:id="rId8" sheetId="9"/>
+    <sheet name="VT-P-DebitVoid-DualCF-Generic" r:id="rId9" sheetId="10"/>
+    <sheet name="VT-C-DebitVoid-NoCF-Generic" r:id="rId10" sheetId="11"/>
+    <sheet name="VT-C-DebitVoid-SingleCF-Generic" r:id="rId11" sheetId="12"/>
+    <sheet name="VT-C-DebitVoid-DualCF-Generic" r:id="rId12" sheetId="13"/>
+    <sheet name="VT-P-DebitCredit-NoCF-Generic" r:id="rId13" sheetId="14"/>
+    <sheet name="VT-P-DebitCredit-SingleCF-Gener" r:id="rId14" sheetId="15"/>
+    <sheet name="VT-P-DebitCredit-DualCF-Generic" r:id="rId15" sheetId="16"/>
+    <sheet name="VT-C-DebitCredit-NoCF-Generic" r:id="rId16" sheetId="17"/>
+    <sheet name="VT-C-DebitCredit-SingleCF-Gener" r:id="rId17" sheetId="18"/>
+    <sheet name="VT-C-DebitCredit-DualCF-Generic" r:id="rId18" sheetId="19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="125">
   <si>
     <t>FirstName</t>
   </si>
@@ -400,12 +400,40 @@
   </si>
   <si>
     <t>4568</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Wed Feb 05 19:31:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 05 21:06:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Wed Feb 05 21:20:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Feb 05 21:27:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Feb 06 16:06:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Feb 06 16:42:05 IST 2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -461,22 +489,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -493,10 +521,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -531,7 +559,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -583,7 +611,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -694,21 +722,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -725,7 +753,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -777,15 +805,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C179FDD-E618-4742-8F86-80396375312B}">
-  <dimension ref="A1:AH5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C179FDD-E618-4742-8F86-80396375312B}">
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
@@ -793,41 +821,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="35" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -1299,8 +1327,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1308,8 +1336,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA039D40-AB89-4825-812F-288703E2DE41}">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA039D40-AB89-4825-812F-288703E2DE41}">
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -1317,40 +1345,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.85546875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="17.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="34" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -1543,7 +1571,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1551,8 +1579,8 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7240EBFC-8352-4A78-9C5F-F61CFDFB11C6}">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7240EBFC-8352-4A78-9C5F-F61CFDFB11C6}">
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -1560,40 +1588,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="40.85546875" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="28.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="27.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="17.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="34" max="16384" style="1" width="40.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -1786,7 +1814,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1794,8 +1822,8 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B5208F-6131-4E8E-B49E-EA4CF7E2AEA8}">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B5208F-6131-4E8E-B49E-EA4CF7E2AEA8}">
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -1803,40 +1831,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="32" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="40.85546875" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="35.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="32.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="17.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="34" max="16384" style="1" width="40.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -2029,7 +2057,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2037,8 +2065,8 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6DA21E-C0FD-406D-B918-6EA9E65DFA51}">
-  <dimension ref="A1:AH5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6DA21E-C0FD-406D-B918-6EA9E65DFA51}">
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
@@ -2046,41 +2074,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="35" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -2552,7 +2580,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2560,8 +2588,8 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36AC063-7B2D-4A8C-BBEE-74EC43C855B0}">
-  <dimension ref="A1:AI5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36AC063-7B2D-4A8C-BBEE-74EC43C855B0}">
+  <dimension ref="A1:AJ5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1:AI5"/>
@@ -2569,41 +2597,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.7109375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="10" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="32.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="9.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="23.7109375" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="35" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -3090,7 +3118,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3098,8 +3126,8 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AA485F-52F2-474B-A028-CB0E8F2BCA2B}">
-  <dimension ref="A1:AH5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AA485F-52F2-474B-A028-CB0E8F2BCA2B}">
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -3107,41 +3135,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.85546875" style="1" customWidth="1"/>
-    <col min="34" max="34" width="8.42578125" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="28.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="8.42578125" collapsed="true"/>
+    <col min="35" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -3613,7 +3641,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3621,8 +3649,8 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0973E4DA-EDA8-4F1C-A4F8-23673FA64EB4}">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0973E4DA-EDA8-4F1C-A4F8-23673FA64EB4}">
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
@@ -3630,40 +3658,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.85546875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="17.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="34" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -3768,6 +3796,12 @@
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>62</v>
       </c>
@@ -3856,7 +3890,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3864,8 +3898,8 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EFF342-4D5E-4066-AB33-FA77D4DA0448}">
-  <dimension ref="A1:AH2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EFF342-4D5E-4066-AB33-FA77D4DA0448}">
+  <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AH21" sqref="AH21"/>
@@ -3873,40 +3907,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="40.85546875" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="28.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="27.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="17.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="34" max="16384" style="1" width="40.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -4014,6 +4048,12 @@
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>62</v>
       </c>
@@ -4105,7 +4145,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4113,8 +4153,8 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819298FE-667E-4491-B43C-4C5F5C5B86A9}">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819298FE-667E-4491-B43C-4C5F5C5B86A9}">
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K41" sqref="K41"/>
@@ -4122,40 +4162,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="32" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="40.85546875" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="35.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="32.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="17.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="34" max="16384" style="1" width="40.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -4260,6 +4300,12 @@
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>62</v>
       </c>
@@ -4348,7 +4394,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4356,8 +4402,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3208BD3-C71F-4161-AC24-4C1B9A477B93}">
-  <dimension ref="A1:AH5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3208BD3-C71F-4161-AC24-4C1B9A477B93}">
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
@@ -4365,41 +4411,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.7109375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="10" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="32.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="9.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="23.7109375" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="35" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -4872,7 +4918,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4880,8 +4926,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE6ED460-B223-4CAB-9191-9A9157FCAFF2}">
-  <dimension ref="A1:AH5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE6ED460-B223-4CAB-9191-9A9157FCAFF2}">
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -4889,41 +4935,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.85546875" style="1" customWidth="1"/>
-    <col min="34" max="34" width="8.42578125" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="28.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="8.42578125" collapsed="true"/>
+    <col min="35" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -5396,7 +5442,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -5404,8 +5450,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5A709C-376A-4BB7-80A3-AEE59337925F}">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5A709C-376A-4BB7-80A3-AEE59337925F}">
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -5413,40 +5459,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.85546875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="17.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="34" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -5639,7 +5685,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -5647,8 +5693,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEB4E4C-40CF-48DE-B706-07F07629C13E}">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEB4E4C-40CF-48DE-B706-07F07629C13E}">
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -5656,40 +5702,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="40.85546875" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="28.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="27.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="17.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="34" max="16384" style="1" width="40.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -5882,8 +5928,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -5891,8 +5937,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8BAD15-65CA-4065-BED2-481F29154B92}">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8BAD15-65CA-4065-BED2-481F29154B92}">
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="A1:XFD1048576"/>
@@ -5900,40 +5946,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="32" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="40.85546875" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="35.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="32.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="17.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="34" max="16384" style="1" width="40.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -6126,7 +6172,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -6134,8 +6180,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2502D5-E039-457F-ADC9-B4319A7A5748}">
-  <dimension ref="A1:AH5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2502D5-E039-457F-ADC9-B4319A7A5748}">
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -6143,41 +6189,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="35" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -6649,7 +6695,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -6657,8 +6703,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C9396A-E44B-451B-A41D-265D0E056BB0}">
-  <dimension ref="A1:AH5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C9396A-E44B-451B-A41D-265D0E056BB0}">
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -6666,41 +6712,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.7109375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="10" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="32.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="33.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="9.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="23.7109375" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="35" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -7172,7 +7218,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -7180,8 +7226,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FFC52F-45D2-442D-9ACA-113B8A078562}">
-  <dimension ref="A1:AH5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FFC52F-45D2-442D-9ACA-113B8A078562}">
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -7189,41 +7235,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.85546875" style="1" customWidth="1"/>
-    <col min="34" max="34" width="8.42578125" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="28.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="8.42578125" collapsed="true"/>
+    <col min="35" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -7695,7 +7741,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>